<commit_message>
Cut dependencies and unused functions; add documentation
</commit_message>
<xml_diff>
--- a/data-ext/example-returns/Merrimack-NH-2016_edits_small.xlsx
+++ b/data-ext/example-returns/Merrimack-NH-2016_edits_small.xlsx
@@ -8,12 +8,14 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="rmerrimack" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="HTML_1" vbProcedure="false">$A$1:$H$9</definedName>
-    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">$A$1:$H$9</definedName>
-    <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">rmerrimack!$A$1:$H$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">rmerrimack!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Titles" vbProcedure="false">rmerrimack!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">rmerrimack!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">rmerrimack!$1:$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +32,7 @@
     <t xml:space="preserve">State of New Hampshire - General Election</t>
   </si>
   <si>
-    <t xml:space="preserve">Merrimack County Offices</t>
+    <t xml:space="preserve">Merrimack County Offices  </t>
   </si>
   <si>
     <t xml:space="preserve">Sheriff</t>
@@ -51,7 +53,7 @@
     <t xml:space="preserve">Murray, r/d</t>
   </si>
   <si>
-    <t xml:space="preserve">Hammond, r</t>
+    <t xml:space="preserve"> Hammond, r</t>
   </si>
   <si>
     <t xml:space="preserve">Rodriguez, d</t>
@@ -76,14 +78,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MMMM\ D&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,18 +110,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="7"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
-      <family val="0"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="7"/>
+      <b val="true"/>
+      <sz val="9"/>
       <name val="Times New Roman"/>
-      <family val="0"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -127,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -136,18 +144,133 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="dotted">
-        <color rgb="FFCCCCCC"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF5C616C"/>
       </left>
-      <right style="dotted">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color rgb="FF5C616C"/>
       </right>
-      <top style="dotted">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
       </top>
-      <bottom style="dotted">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF5C616C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5C616C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FF5C616C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thick">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5C616C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5C616C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thick">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5C616C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF5C616C"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF5C616C"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -170,39 +293,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="9" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -230,7 +439,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -262,7 +471,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5C616C"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -282,220 +491,362 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="9" style="1" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="8.84"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+    <row r="3" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>42682</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+    <row r="4" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="16" t="n">
         <v>2035</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="18" t="n">
         <v>2013</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="20" t="n">
         <v>1296</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="16" t="n">
         <v>699</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="16" t="n">
         <v>1310</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="18" t="n">
         <v>1277</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="5" t="n">
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="n">
         <v>714</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="16" t="n">
         <v>564</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="16" t="n">
         <v>1661</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="18" t="n">
         <v>1618</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="20" t="n">
         <v>988</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="16" t="n">
         <v>602</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="21" t="n">
         <v>4585</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="22" t="n">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="18" t="n">
         <v>4481</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="20" t="n">
         <v>2672</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="16" t="n">
         <v>1840</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="24" t="n">
+        <f aca="false">SUM(B5:B8)</f>
         <v>9591</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="17" t="n">
+        <f aca="false">SUM(C5:C8)</f>
         <v>34</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="25" t="n">
+        <f aca="false">SUM(D5:D8)</f>
         <v>9389</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="26" t="n">
+        <f aca="false">SUM(E5:E8)</f>
         <v>28</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="27" t="n">
+        <f aca="false">SUM(F5:F8)</f>
         <v>5670</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="16" t="n">
+        <f aca="false">SUM(G5:G8)</f>
         <v>3705</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="4" t="n">
+        <f aca="false">SUM(H5:H8)</f>
         <v>6</v>
       </c>
     </row>
+    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:H3"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.25" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>